<commit_message>
Edit some lines in file excel
</commit_message>
<xml_diff>
--- a/NUnit_53_57_HauNgoc/UnitTest_53_57_HauNgoc/Data_53_57_HauNgoc/DataDriver_53_57_HauNgoc.xlsx
+++ b/NUnit_53_57_HauNgoc/UnitTest_53_57_HauNgoc/Data_53_57_HauNgoc/DataDriver_53_57_HauNgoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KiemThuPhanMem\KiemThuPhanMem\NUnit_53_57_HauNgoc\UnitTest_53_57_HauNgoc\Data_53_57_HauNgoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED698F08-CA18-423C-B328-0CB113FED650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75A2555-AF67-497A-89E3-50C352415E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="996" yWindow="876" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,10 +422,10 @@
         <v>0</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>15</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -551,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>-10</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>

</xml_diff>